<commit_message>
Kozterulet atvezetese az adatbazisba
</commit_message>
<xml_diff>
--- a/szakmaiGyakorlatDokumentacio/Kivitelezes/xls-csv/kozteruletjellege.xlsx
+++ b/szakmaiGyakorlatDokumentacio/Kivitelezes/xls-csv/kozteruletjellege.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\InfGit\ambulanc\szakmaiGyakorlatDokumentacio\Kivitelezes\xls-csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD3F0245-3FF8-4472-A574-341FDC370AE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1084E286-FB24-46C0-ADA0-0C33F17B383B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15750" xr2:uid="{FCDF63DD-DDB4-48BC-8530-9F0E519FFD3C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Jelleg</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>üdülőpart</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -493,196 +496,307 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1725895D-294C-4036-A236-39C6D5C28EE1}">
-  <dimension ref="A1:A37"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="B28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="B30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="B32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="B33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="B34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="B35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="B36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>